<commit_message>
zero-erp to alter activity-rule.xlsx
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-erp/src/main/resources/plugin/erp/oob/rule/process.vendor.assessment/activity-rule.xlsx
+++ b/vertx-pin/zero-erp/src/main/resources/plugin/erp/oob/rule/process.vendor.assessment/activity-rule.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-erp/src/main/resources/plugin/erp/oob/rule/process.vendor.assessment/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFE43BE-591B-3045-9DC7-30E90F143B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="52140" yWindow="-6560" windowWidth="47800" windowHeight="23220" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="52140" yWindow="-6564" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-CDATA" sheetId="7" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -302,10 +296,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>e.init</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>处理/关闭</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -430,13 +420,17 @@
   </si>
   <si>
     <t>cf79a1f3-da65-4b42-8c5c-b927c07ee47b</t>
+  </si>
+  <si>
+    <t>e.adjust</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -651,7 +645,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -709,7 +703,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -761,7 +755,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -955,42 +949,42 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500280C7-B0AC-7C45-9420-F2551253A777}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.36328125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="111" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="94.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="2"/>
+    <col min="12" max="12" width="18.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="94.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -1014,7 +1008,7 @@
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1064,7 +1058,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1114,12 +1108,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>31</v>
@@ -1143,7 +1137,7 @@
         <v>34</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="11" t="b">
@@ -1151,17 +1145,17 @@
       </c>
       <c r="M5" s="11"/>
       <c r="N5" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>36</v>
@@ -1185,7 +1179,7 @@
         <v>34</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="11" t="b">
@@ -1193,17 +1187,17 @@
       </c>
       <c r="M6" s="11"/>
       <c r="N6" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>31</v>
@@ -1227,7 +1221,7 @@
         <v>34</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="11" t="b">
@@ -1235,17 +1229,17 @@
       </c>
       <c r="M7" s="11"/>
       <c r="N7" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>31</v>
@@ -1269,7 +1263,7 @@
         <v>34</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="11" t="b">
@@ -1277,17 +1271,17 @@
       </c>
       <c r="M8" s="11"/>
       <c r="N8" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>31</v>
@@ -1311,7 +1305,7 @@
         <v>34</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="11" t="b">
@@ -1319,17 +1313,17 @@
       </c>
       <c r="M9" s="11"/>
       <c r="N9" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>31</v>
@@ -1353,7 +1347,7 @@
         <v>34</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="11" t="b">
@@ -1361,17 +1355,17 @@
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>36</v>
@@ -1386,7 +1380,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>62</v>
@@ -1395,7 +1389,7 @@
         <v>34</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="11" t="b">
@@ -1403,17 +1397,17 @@
       </c>
       <c r="M11" s="11"/>
       <c r="N11" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>36</v>
@@ -1425,10 +1419,10 @@
         <v>1010</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H12" s="11" t="s">
         <v>61</v>
@@ -1437,7 +1431,7 @@
         <v>34</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="11" t="b">
@@ -1445,17 +1439,17 @@
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>36</v>
@@ -1470,7 +1464,7 @@
         <v>46</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>63</v>
@@ -1479,7 +1473,7 @@
         <v>34</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K13" s="11" t="s">
         <v>41</v>
@@ -1489,17 +1483,17 @@
       </c>
       <c r="M13" s="11"/>
       <c r="N13" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>36</v>
@@ -1523,7 +1517,7 @@
         <v>34</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="11" t="b">
@@ -1531,17 +1525,17 @@
       </c>
       <c r="M14" s="11"/>
       <c r="N14" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>36</v>
@@ -1565,7 +1559,7 @@
         <v>34</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="11" t="b">
@@ -1573,17 +1567,17 @@
       </c>
       <c r="M15" s="11"/>
       <c r="N15" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>44</v>
@@ -1595,19 +1589,19 @@
         <v>1005</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>34</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="11" t="b">
@@ -1615,17 +1609,17 @@
       </c>
       <c r="M16" s="11"/>
       <c r="N16" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>44</v>
@@ -1649,7 +1643,7 @@
         <v>34</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="11" t="b">
@@ -1657,17 +1651,17 @@
       </c>
       <c r="M17" s="11"/>
       <c r="N17" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>44</v>
@@ -1691,7 +1685,7 @@
         <v>34</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K18" s="11" t="s">
         <v>41</v>
@@ -1701,17 +1695,17 @@
       </c>
       <c r="M18" s="11"/>
       <c r="N18" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>44</v>
@@ -1735,7 +1729,7 @@
         <v>34</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="11" t="b">
@@ -1743,17 +1737,17 @@
       </c>
       <c r="M19" s="11"/>
       <c r="N19" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>44</v>
@@ -1777,7 +1771,7 @@
         <v>34</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="11" t="b">
@@ -1785,20 +1779,20 @@
       </c>
       <c r="M20" s="11"/>
       <c r="N20" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O20" s="11"/>
       <c r="P20" s="11"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>49</v>
@@ -1807,19 +1801,19 @@
         <v>1005</v>
       </c>
       <c r="F21" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="H21" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>34</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="11" t="b">
@@ -1827,20 +1821,20 @@
       </c>
       <c r="M21" s="11"/>
       <c r="N21" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>49</v>
@@ -1849,7 +1843,7 @@
         <v>1010</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>64</v>
@@ -1861,7 +1855,7 @@
         <v>34</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="11" t="b">
@@ -1869,20 +1863,20 @@
       </c>
       <c r="M22" s="11"/>
       <c r="N22" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O22" s="11"/>
       <c r="P22" s="11"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>35</v>
@@ -1903,7 +1897,7 @@
         <v>34</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K23" s="11" t="s">
         <v>41</v>
@@ -1913,20 +1907,20 @@
       </c>
       <c r="M23" s="11"/>
       <c r="N23" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O23" s="11"/>
       <c r="P23" s="11"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>49</v>
@@ -1947,7 +1941,7 @@
         <v>34</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K24" s="9"/>
       <c r="L24" s="11" t="b">
@@ -1955,20 +1949,20 @@
       </c>
       <c r="M24" s="11"/>
       <c r="N24" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>49</v>
@@ -1989,7 +1983,7 @@
         <v>34</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="11" t="b">
@@ -1997,20 +1991,20 @@
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>49</v>
@@ -2019,19 +2013,19 @@
         <v>1020</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>66</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>34</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="11" t="b">
@@ -2039,7 +2033,7 @@
       </c>
       <c r="M26" s="11"/>
       <c r="N26" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O26" s="11"/>
       <c r="P26" s="11"/>

</xml_diff>